<commit_message>
Enhance CSV and XLSX execution substrates with ampersand normalization and update test results
This commit introduces a new function to normalize ampersand operators in formulas for both CSV and XLSX execution substrates, ensuring consistent spacing around ampersands while respecting string boundaries. Additionally, the test results have been updated to reflect a perfect pass rate of 100% across all evaluated fields, showcasing improved accuracy in the evaluation framework. These changes aim to enhance the clarity and usability of the evaluation process across all substrates.
</commit_message>
<xml_diff>
--- a/execution-substrates/csv/rulebook.xlsx
+++ b/execution-substrates/csv/rulebook.xlsx
@@ -644,7 +644,7 @@
       </c>
       <c r="I2" s="3" t="inlineStr">
         <is>
-          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held</t>
+          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held, Has no Identity</t>
         </is>
       </c>
       <c r="J2" s="3" t="n"/>
@@ -738,7 +738,7 @@
       </c>
       <c r="I3" s="3" t="inlineStr">
         <is>
-          <t>No Syntax &amp; No Parsing Neede &amp; Is the Thing &amp; No Decoding Pressure &amp; No AST, Not 'Ontology' AND Can Be Held</t>
+          <t>No Syntax &amp; No Parsing Neede &amp; Is the Thing &amp; No Decoding Pressure &amp; No AST, Not 'Ontology' AND Can Be Held, Has Identity</t>
         </is>
       </c>
       <c r="J3" s="3" t="n"/>
@@ -832,7 +832,7 @@
       </c>
       <c r="I4" s="3" t="inlineStr">
         <is>
-          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held</t>
+          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held, Has no Identity</t>
         </is>
       </c>
       <c r="J4" s="3" t="n"/>
@@ -926,7 +926,7 @@
       </c>
       <c r="I5" s="3" t="inlineStr">
         <is>
-          <t>No Syntax &amp; Requires Parsing &amp; Is the Thing &amp; No Decoding Pressure &amp; No AST, Not 'Ontology' AND Can't Be Held</t>
+          <t>No Syntax &amp; Requires Parsing &amp; Is the Thing &amp; No Decoding Pressure &amp; No AST, Not 'Ontology' AND Can't Be Held, Has Identity</t>
         </is>
       </c>
       <c r="J5" s="3" t="n"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="I6" s="3" t="inlineStr">
         <is>
-          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held</t>
+          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held, Has no Identity</t>
         </is>
       </c>
       <c r="J6" s="3" t="n"/>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="I7" s="3" t="inlineStr">
         <is>
-          <t>No Syntax &amp; No Parsing Neede &amp; Describes the thing &amp; No Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held</t>
+          <t>No Syntax &amp; No Parsing Neede &amp; Describes the thing &amp; No Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held, Has Identity</t>
         </is>
       </c>
       <c r="J7" s="3" t="n"/>
@@ -1208,7 +1208,7 @@
       </c>
       <c r="I8" s="3" t="inlineStr">
         <is>
-          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held</t>
+          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held, Has no Identity</t>
         </is>
       </c>
       <c r="J8" s="3" t="n"/>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="I9" s="3" t="inlineStr">
         <is>
-          <t>No Syntax &amp; Requires Parsing &amp; Is the Thing &amp; No Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can Be Held</t>
+          <t>No Syntax &amp; Requires Parsing &amp; Is the Thing &amp; No Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can Be Held, Has Identity</t>
         </is>
       </c>
       <c r="J9" s="3" t="inlineStr">
@@ -1400,7 +1400,7 @@
       </c>
       <c r="I10" s="3" t="inlineStr">
         <is>
-          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held</t>
+          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held, Has no Identity</t>
         </is>
       </c>
       <c r="J10" s="3" t="inlineStr">
@@ -1498,7 +1498,7 @@
       </c>
       <c r="I11" s="3" t="inlineStr">
         <is>
-          <t>No Syntax &amp; No Parsing Neede &amp; Is the Thing &amp; Has Linear Decoding Pressure &amp; No AST, Not 'Ontology' AND Can Be Held</t>
+          <t>No Syntax &amp; No Parsing Neede &amp; Is the Thing &amp; Has Linear Decoding Pressure &amp; No AST, Not 'Ontology' AND Can Be Held, Has Identity</t>
         </is>
       </c>
       <c r="J11" s="3" t="n"/>
@@ -1592,7 +1592,7 @@
       </c>
       <c r="I12" s="3" t="inlineStr">
         <is>
-          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held</t>
+          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held, Has no Identity</t>
         </is>
       </c>
       <c r="J12" s="3" t="n"/>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="I13" s="3" t="inlineStr">
         <is>
-          <t>No Syntax &amp; Requires Parsing &amp; Is the Thing &amp; Has Linear Decoding Pressure &amp; No AST, Not 'Ontology' AND Can't Be Held</t>
+          <t>No Syntax &amp; Requires Parsing &amp; Is the Thing &amp; Has Linear Decoding Pressure &amp; No AST, Not 'Ontology' AND Can't Be Held, Has Identity</t>
         </is>
       </c>
       <c r="J13" s="3" t="n"/>
@@ -1780,7 +1780,7 @@
       </c>
       <c r="I14" s="3" t="inlineStr">
         <is>
-          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held</t>
+          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held, Has no Identity</t>
         </is>
       </c>
       <c r="J14" s="3" t="n"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="I15" s="3" t="inlineStr">
         <is>
-          <t>No Syntax &amp; No Parsing Neede &amp; Is the Thing &amp; No Decoding Pressure &amp; Resolves to AST, Not 'Ontology' AND Can't Be Held</t>
+          <t>No Syntax &amp; No Parsing Neede &amp; Is the Thing &amp; No Decoding Pressure &amp; Resolves to AST, Not 'Ontology' AND Can't Be Held, Has no Identity</t>
         </is>
       </c>
       <c r="J15" s="3" t="n"/>
@@ -1968,7 +1968,7 @@
       </c>
       <c r="I16" s="3" t="inlineStr">
         <is>
-          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held</t>
+          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held, Has no Identity</t>
         </is>
       </c>
       <c r="J16" s="3" t="n"/>
@@ -2062,7 +2062,7 @@
       </c>
       <c r="I17" s="3" t="inlineStr">
         <is>
-          <t>No Syntax &amp; No Parsing Neede &amp; Is the Thing &amp; No Decoding Pressure &amp; No AST, Is Stable Ontology AND Can't Be Held</t>
+          <t>No Syntax &amp; No Parsing Neede &amp; Is the Thing &amp; No Decoding Pressure &amp; No AST, Is Stable Ontology AND Can't Be Held, Has no Identity</t>
         </is>
       </c>
       <c r="J17" s="3" t="n"/>
@@ -2156,7 +2156,7 @@
       </c>
       <c r="I18" s="3" t="inlineStr">
         <is>
-          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held</t>
+          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held, Has no Identity</t>
         </is>
       </c>
       <c r="J18" s="3" t="n"/>
@@ -2250,7 +2250,7 @@
       </c>
       <c r="I19" s="3" t="inlineStr">
         <is>
-          <t>No Syntax &amp; Requires Parsing &amp; Is the Thing &amp; No Decoding Pressure &amp; Resolves to AST, Not 'Ontology' AND Can Be Held</t>
+          <t>No Syntax &amp; Requires Parsing &amp; Is the Thing &amp; No Decoding Pressure &amp; Resolves to AST, Not 'Ontology' AND Can Be Held, Has Identity</t>
         </is>
       </c>
       <c r="J19" s="3" t="n"/>
@@ -2344,7 +2344,7 @@
       </c>
       <c r="I20" s="3" t="inlineStr">
         <is>
-          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held</t>
+          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held, Has no Identity</t>
         </is>
       </c>
       <c r="J20" s="3" t="n"/>
@@ -2438,7 +2438,7 @@
       </c>
       <c r="I21" s="3" t="inlineStr">
         <is>
-          <t>No Syntax &amp; No Parsing Neede &amp; Is the Thing &amp; No Decoding Pressure &amp; No AST, Is Stable Ontology AND Can Be Held</t>
+          <t>No Syntax &amp; No Parsing Neede &amp; Is the Thing &amp; No Decoding Pressure &amp; No AST, Is Stable Ontology AND Can Be Held, Has Identity</t>
         </is>
       </c>
       <c r="J21" s="3" t="n"/>
@@ -2532,7 +2532,7 @@
       </c>
       <c r="I22" s="3" t="inlineStr">
         <is>
-          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held</t>
+          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held, Has no Identity</t>
         </is>
       </c>
       <c r="J22" s="3" t="n"/>
@@ -2626,7 +2626,7 @@
       </c>
       <c r="I23" s="3" t="inlineStr">
         <is>
-          <t>No Syntax &amp; Requires Parsing &amp; Is the Thing &amp; No Decoding Pressure &amp; Resolves to AST, Not 'Ontology' AND Can't Be Held</t>
+          <t>No Syntax &amp; Requires Parsing &amp; Is the Thing &amp; No Decoding Pressure &amp; Resolves to AST, Not 'Ontology' AND Can't Be Held, Has Identity</t>
         </is>
       </c>
       <c r="J23" s="3" t="n"/>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="I24" s="3" t="inlineStr">
         <is>
-          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held</t>
+          <t>Has Syntax &amp; Requires Parsing &amp; Describes the thing &amp; Has Linear Decoding Pressure &amp; Resolves to AST, Is Stable Ontology AND Can't Be Held, Has no Identity</t>
         </is>
       </c>
       <c r="J24" s="3" t="inlineStr">

</xml_diff>